<commit_message>
Removed unused methods Updated TestData
</commit_message>
<xml_diff>
--- a/APITesting/DataAccess/TestData.xlsx
+++ b/APITesting/DataAccess/TestData.xlsx
@@ -142,15 +142,9 @@
     <t xml:space="preserve">MSPCreateCustomerPost_UAE</t>
   </si>
   <si>
-    <t xml:space="preserve">Authorization:osnAuth osnauth_x_application_id=6,  osnauth_x_source_id=14, osnauth_x_timestamp=1546941635, osnauth_x_signature=Y2I3YmU1Zjc4NTBiZTk0Yzk2NGUxNjkxY2NlYWMwYjBkNDllNzdjNDEyYThjNTgxZTU5NzI3NjYxODY2ZWNjYg==</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"e4cbf1c2-2bdb-4059-9517-95ad401e2e37","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-08T10:10:00.7989349+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{"UserId":"00212029-ba97-468f-b670-b21eb2a93a8e",
 "EmailAddress":"info@osn.com",
-"MobileNumber":"96558880449075",
+"MobileNumber":"96558880449081",
 "Packages":[  
    3507
 ],
@@ -175,13 +169,19 @@
 "ExpiryDate":"2023-12-12T13:00:54.415093Z"}</t>
   </si>
   <si>
-    <t xml:space="preserve">{"MobileNumber" : "97110001008", "EmailAddress" : "autoexection@osn.com", "Packages" : [3507], "Password" : "413703","extra": { "MCC": "971","MNC": "01","Prod": "01"}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"67875a2c-c6f6-44c2-8e92-37eb51ba67fe","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-08T10:10:52.1351324+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"50429766-21fe-4a66-8f1d-4e13bb2182f5","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-08T10:10:53.8445301+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+    <t xml:space="preserve">{"userId":"18823fc7-5cf8-4d0d-94ce-0c542f34c748","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-09T05:13:50.420393+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"MobileNumber" : "971569143419", "EmailAddress" : "autoexection@osn.com", "Packages" : [3507], "Password" : "413703","extra": { "MCC": "971","MNC": "01","Prod": "01"}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorization:osnAuth osnauth_x_application_id=6,  osnauth_x_source_id=14, osnauth_x_timestamp=1547012791, osnauth_x_signature=M2IxNTM4ZTU3NjRhNTk3OWRiYTA1YjI4Zjc3NDkxOTVlNmEwNjgxZWExNTc2M2Q4ZTE5MDA4ZDkzYjVhY2RhYg==</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"userId":"ef99562c-4818-4c0c-804c-0b3fd08b9093","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-09T05:47:35.8289384+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"userId":"90900888-eb50-45b9-978b-5747c6dcf71b","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-09T06:04:52.238623+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
   </si>
 </sst>
 </file>
@@ -519,8 +519,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -596,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>36</v>
@@ -620,16 +620,16 @@
         <v>11</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
@@ -695,13 +695,13 @@
         <v>11</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
-Removed Recordcount, Key and added functionality to TcId -Added primaryKey in Model -Chnages to Data access for fetching TC's and steps -Removed of key and record cound updaed to DataSheet
</commit_message>
<xml_diff>
--- a/APITesting/DataAccess/TestData.xlsx
+++ b/APITesting/DataAccess/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t xml:space="preserve">TcName</t>
   </si>
@@ -46,12 +46,6 @@
     <t xml:space="preserve">RequestMethod</t>
   </si>
   <si>
-    <t xml:space="preserve">Validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://xf0lv66uc8.execute-api.eu-west-1.amazonaws.com</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t xml:space="preserve">ApiResponse</t>
   </si>
   <si>
-    <t xml:space="preserve">1,ApiResponse</t>
-  </si>
-  <si>
     <t xml:space="preserve">DataToValidate</t>
   </si>
   <si>
@@ -130,9 +121,6 @@
     <t xml:space="preserve">Validate the Response for MSP Create customer</t>
   </si>
   <si>
-    <t xml:space="preserve">3,ApiResponse</t>
-  </si>
-  <si>
     <t xml:space="preserve">Headers</t>
   </si>
   <si>
@@ -140,11 +128,32 @@
   </si>
   <si>
     <t xml:space="preserve">MSPCreateCustomerPost_UAE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1,ApiResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1,ApiResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fieldsToValidate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"userId":"2f93085e-12c5-4f97-99ab-0161b6cb8e94","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T10:25:40.8107238+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"userId":"aa9ad10c-eb00-43b6-9c83-f42c4fa34624","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T10:25:42.0509605+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorization:osnAuth osnauth_x_application_id=6,  osnauth_x_source_id=14, osnauth_x_timestamp=1547124679, osnauth_x_signature=YjVmOWQ5ODI3NWZiYmJjZGU3NGJhMDAwODg3OTVmODExM2RjNGUzZmQxOWY3YjczNjRkZDBkYTljMTM5NDYxZA==</t>
   </si>
   <si>
     <t xml:space="preserve">{"UserId":"00212029-ba97-468f-b670-b21eb2a93a8e",
 "EmailAddress":"info@osn.com",
-"MobileNumber":"96558880449081",
+"MobileNumber":"9651000221",
 "Packages":[  
    3507
 ],
@@ -169,19 +178,13 @@
 "ExpiryDate":"2023-12-12T13:00:54.415093Z"}</t>
   </si>
   <si>
-    <t xml:space="preserve">{"userId":"18823fc7-5cf8-4d0d-94ce-0c542f34c748","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-09T05:13:50.420393+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"MobileNumber" : "971569143419", "EmailAddress" : "autoexection@osn.com", "Packages" : [3507], "Password" : "413703","extra": { "MCC": "971","MNC": "01","Prod": "01"}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authorization:osnAuth osnauth_x_application_id=6,  osnauth_x_source_id=14, osnauth_x_timestamp=1547012791, osnauth_x_signature=M2IxNTM4ZTU3NjRhNTk3OWRiYTA1YjI4Zjc3NDkxOTVlNmEwNjgxZWExNTc2M2Q4ZTE5MDA4ZDkzYjVhY2RhYg==</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"ef99562c-4818-4c0c-804c-0b3fd08b9093","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-09T05:47:35.8289384+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"90900888-eb50-45b9-978b-5747c6dcf71b","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-09T06:04:52.238623+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+    <t xml:space="preserve">{"MobileNumber" : "9711000222", "EmailAddress" : "autoexection@osn.com", "Packages" : [3507], "Password" : "413703","extra": { "MCC": "971","MNC": "01","Prod": "01"}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"userId":"31010bef-7c4b-431a-84bf-ff3ea023e735","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T12:52:16.4571777+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"userId":"3189ed23-61ca-44b6-a99a-202c2932dc25","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T12:52:18.265651+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
   </si>
 </sst>
 </file>
@@ -226,14 +229,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -517,231 +519,217 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="2"/>
-    <col min="4" max="6" width="18.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="54.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="53.42578125" style="2" customWidth="1"/>
-    <col min="14" max="15" width="48.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="50.140625" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="5" width="18.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="54.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53.42578125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="48.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="50.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="375">
+      <c r="A2" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" ht="60">
+      <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="150">
+      <c r="A4" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="60">
+      <c r="A5" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="375">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="O5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" ht="60">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="60">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" ht="60">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="portrait" r:id="rId3"/>
@@ -760,13 +748,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -774,10 +762,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -785,10 +773,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -796,10 +784,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -807,10 +795,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -818,10 +806,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved code. No change in functionality
</commit_message>
<xml_diff>
--- a/APITesting/DataAccess/TestData.xlsx
+++ b/APITesting/DataAccess/TestData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="1"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC500391-937D-40BC-B605-88180D12BD31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" fullPrecision="1" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
+  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures">
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
@@ -26,134 +27,131 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
-  <si>
-    <t xml:space="preserve">TcName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DataModel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RequestMethod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://xf0lv66uc8.execute-api.eu-west-1.amazonaws.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Dev/create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CreateRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customerType:=:OTT Telco|customerStatus:=:OTT Active|accountType:=:OTT Msp|agreementType:NOTEMPTY:NA|productId:=:3599|productStatus:=:430|responseCode:=:0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCnAMe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run Fkag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asfasd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">afasf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RunFlag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TcId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RunAPIRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BaseUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ValidateApiResponse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ApiResponse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DataToValidate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run MSP Create customer API request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate the Response for MSP Create customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Headers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSPCreateCustomerPost_Kuwait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSPCreateCustomerPost_UAE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1,ApiResponse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1,ApiResponse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fieldsToValidate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"2f93085e-12c5-4f97-99ab-0161b6cb8e94","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T10:25:40.8107238+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"aa9ad10c-eb00-43b6-9c83-f42c4fa34624","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T10:25:42.0509605+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authorization:osnAuth osnauth_x_application_id=6,  osnauth_x_source_id=14, osnauth_x_timestamp=1547124679, osnauth_x_signature=YjVmOWQ5ODI3NWZiYmJjZGU3NGJhMDAwODg3OTVmODExM2RjNGUzZmQxOWY3YjczNjRkZDBkYTljMTM5NDYxZA==</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"UserId":"00212029-ba97-468f-b670-b21eb2a93a8e",
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+  <si>
+    <t>TcName</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>DataModel</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>RequestMethod</t>
+  </si>
+  <si>
+    <t>https://xf0lv66uc8.execute-api.eu-west-1.amazonaws.com</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/Dev/create</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>CreateRequest</t>
+  </si>
+  <si>
+    <t>customerType:=:OTT Telco|customerStatus:=:OTT Active|accountType:=:OTT Msp|agreementType:NOTEMPTY:NA|productId:=:3599|productStatus:=:430|responseCode:=:0</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>TCnAMe</t>
+  </si>
+  <si>
+    <t>Run Fkag</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>asfasd</t>
+  </si>
+  <si>
+    <t>afasf</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>RunFlag</t>
+  </si>
+  <si>
+    <t>TcId</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>RunAPIRequest</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>BaseUrl</t>
+  </si>
+  <si>
+    <t>ValidateApiResponse</t>
+  </si>
+  <si>
+    <t>ApiResponse</t>
+  </si>
+  <si>
+    <t>DataToValidate</t>
+  </si>
+  <si>
+    <t>Run MSP Create customer API request</t>
+  </si>
+  <si>
+    <t>Validate the Response for MSP Create customer</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>MSPCreateCustomerPost_Kuwait</t>
+  </si>
+  <si>
+    <t>MSPCreateCustomerPost_UAE</t>
+  </si>
+  <si>
+    <t>1.1,ApiResponse</t>
+  </si>
+  <si>
+    <t>2.1,ApiResponse</t>
+  </si>
+  <si>
+    <t>fieldsToValidate</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>{"userId":"31010bef-7c4b-431a-84bf-ff3ea023e735","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T12:52:16.4571777+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+  </si>
+  <si>
+    <t>{"userId":"3189ed23-61ca-44b6-a99a-202c2932dc25","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T12:52:18.265651+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+  </si>
+  <si>
+    <t>{"UserId":"00212029-ba97-468f-b670-b21eb2a93a8e",
 "EmailAddress":"info@osn.com",
-"MobileNumber":"9651000221",
+"MobileNumber":"9651000223",
 "Packages":[  
    3507
 ],
@@ -178,20 +176,17 @@
 "ExpiryDate":"2023-12-12T13:00:54.415093Z"}</t>
   </si>
   <si>
-    <t xml:space="preserve">{"MobileNumber" : "9711000222", "EmailAddress" : "autoexection@osn.com", "Packages" : [3507], "Password" : "413703","extra": { "MCC": "971","MNC": "01","Prod": "01"}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"31010bef-7c4b-431a-84bf-ff3ea023e735","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T12:52:16.4571777+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"userId":"3189ed23-61ca-44b6-a99a-202c2932dc25","customerType":"OTT Telco","customerStatus":"OTT Active","accountCollection":[{"accountType":"OTT Msp","agreementCollection":[{"agreementType":877,"productCollection":[{"productId":3599,"productStatus":430,"productExpiry":"2069-01-10T12:52:18.265651+00:00"}]}]}],"responseCode":0,"returnId":0,"messageResponse":{"messageCode":0,"exceptionCode":0,"userMessages":null}}</t>
+    <t>{"MobileNumber" : "9711000224", "EmailAddress" : "autoexection@osn.com", "Packages" : [3507], "Password" : "413703","extra": { "MCC": "971","MNC": "01","Prod": "01"}}</t>
+  </si>
+  <si>
+    <t>Authorization:osnAuth osnauth_x_application_id=6,  osnauth_x_source_id=14, osnauth_x_timestamp=1547128136, osnauth_x_signature=ZjQ5NWEzYTM2ODE5MzJmN2UxOTcwM2UxNmQyMDE4YWU3MGM0MGM4ZjM5YjQxY2VhNTRkMDBhODJlZTdiNjUzMw==</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,7 +195,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -226,17 +221,17 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -245,11 +240,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -517,15 +512,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="9.140625" style="2"/>
@@ -541,7 +536,7 @@
     <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
@@ -588,7 +583,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="375">
+    <row r="2" spans="1:15" ht="375" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -617,21 +612,21 @@
         <v>9</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="60">
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>37</v>
       </c>
@@ -657,7 +652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="150">
+    <row r="4" spans="1:15" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2.1</v>
       </c>
@@ -686,21 +681,21 @@
         <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="60">
+    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -728,8 +723,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="portrait" r:id="rId3"/>
@@ -737,16 +732,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -757,7 +752,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -768,7 +763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -779,7 +774,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -790,7 +785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -801,7 +796,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>